<commit_message>
fix(pipelining): fix FLOAD instruction following the LoadStore instruction #2
</commit_message>
<xml_diff>
--- a/programs/fpumaclaurinprogramsinpiover2-32bits.xlsx
+++ b/programs/fpumaclaurinprogramsinpiover2-32bits.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vacla\Projects\cpu\programs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AE0B48-C7EF-4BAD-B3EA-488792A6B10A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0AA506-E01C-41B6-88F3-37F0CFA763AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E410B2C1-F054-41C4-A96D-F1120FBD95E0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E410B2C1-F054-41C4-A96D-F1120FBD95E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Code" sheetId="1" r:id="rId1"/>
@@ -861,8 +861,8 @@
   <dimension ref="A1:Y83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S81" sqref="S81"/>
+      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1326,7 +1326,7 @@
         <v>0</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -1360,7 +1360,7 @@
       </c>
       <c r="S11" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>347</v>
+        <v>747</v>
       </c>
       <c r="T11" t="s">
         <v>87</v>
@@ -1417,14 +1417,14 @@
         <v>1</v>
       </c>
       <c r="Q12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S12" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>B44</v>
+        <v>B47</v>
       </c>
       <c r="T12" t="s">
         <v>89</v>
@@ -1450,7 +1450,7 @@
         <v>1</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -1487,7 +1487,7 @@
       </c>
       <c r="S13" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>1380</v>
+        <v>1B80</v>
       </c>
       <c r="T13" t="s">
         <v>93</v>
@@ -1864,7 +1864,7 @@
         <v>1</v>
       </c>
       <c r="S19" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>DEC2HEX(C19*2^15 + D19*2^14 + E19*2^13 + F19*2^12 + G19*2^11 + H19*2^10 + I19*2^9 + J19*2^8 + K19*2^7 + L19*2^6 + M19*2^5 + N19*2^4 + O19 * 2 ^ 3 + P19  * 2^2 + Q19 * 2 + R19)</f>
         <v>1B01</v>
       </c>
       <c r="T19" t="s">
@@ -4866,6 +4866,21 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N2:R2"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="K3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="A8:V8"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="Q7:R7"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="M4:P4"/>
     <mergeCell ref="I6:J6"/>
@@ -4876,21 +4891,6 @@
     <mergeCell ref="I5:R5"/>
     <mergeCell ref="C6:F6"/>
     <mergeCell ref="G6:H6"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="A8:V8"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N2:R2"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="K3:N3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:R3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5088,7 +5088,7 @@
       </c>
       <c r="C4" t="str">
         <f>Code!S11</f>
-        <v>347</v>
+        <v>747</v>
       </c>
       <c r="E4" t="s">
         <v>51</v>
@@ -5110,7 +5110,7 @@
       </c>
       <c r="C5" t="str">
         <f>Code!S12</f>
-        <v>B44</v>
+        <v>B47</v>
       </c>
       <c r="F5" t="s">
         <v>51</v>

</xml_diff>

<commit_message>
feat(fpu): add calculating up to the term 1/7! #2
</commit_message>
<xml_diff>
--- a/programs/fpumaclaurinprogramsinpiover2-32bits.xlsx
+++ b/programs/fpumaclaurinprogramsinpiover2-32bits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vacla\Projects\cpu\programs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D894CB-81FB-42C5-870D-34477C3F43BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE0E5BD-F5B8-43AF-8054-B93BAB91356E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E410B2C1-F054-41C4-A96D-F1120FBD95E0}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="187">
   <si>
     <t>Hex</t>
   </si>
@@ -473,6 +473,129 @@
   </si>
   <si>
     <t>0x034</t>
+  </si>
+  <si>
+    <t>MOV R3, #A ROR 0</t>
+  </si>
+  <si>
+    <t>MOV R1, #8 ROR 0</t>
+  </si>
+  <si>
+    <t>0x035</t>
+  </si>
+  <si>
+    <t>0x036</t>
+  </si>
+  <si>
+    <t>0x037</t>
+  </si>
+  <si>
+    <t>0x038</t>
+  </si>
+  <si>
+    <t>0x039</t>
+  </si>
+  <si>
+    <t>0x040</t>
+  </si>
+  <si>
+    <t>0x041</t>
+  </si>
+  <si>
+    <t>0x042</t>
+  </si>
+  <si>
+    <t>0x043</t>
+  </si>
+  <si>
+    <t>0x044</t>
+  </si>
+  <si>
+    <t>0x045</t>
+  </si>
+  <si>
+    <t>0x046</t>
+  </si>
+  <si>
+    <t>0x047</t>
+  </si>
+  <si>
+    <t>0x048</t>
+  </si>
+  <si>
+    <t>0x049</t>
+  </si>
+  <si>
+    <t>0x050</t>
+  </si>
+  <si>
+    <t>0x051</t>
+  </si>
+  <si>
+    <t>0x052</t>
+  </si>
+  <si>
+    <t>0x053</t>
+  </si>
+  <si>
+    <t>0x054</t>
+  </si>
+  <si>
+    <t>0x055</t>
+  </si>
+  <si>
+    <t>0x056</t>
+  </si>
+  <si>
+    <t>0x057</t>
+  </si>
+  <si>
+    <t>0x058</t>
+  </si>
+  <si>
+    <t>0x059</t>
+  </si>
+  <si>
+    <t>0x03A</t>
+  </si>
+  <si>
+    <t>0x03B</t>
+  </si>
+  <si>
+    <t>0x03C</t>
+  </si>
+  <si>
+    <t>0x03D</t>
+  </si>
+  <si>
+    <t>0x03E</t>
+  </si>
+  <si>
+    <t>0x03F</t>
+  </si>
+  <si>
+    <t>0x04A</t>
+  </si>
+  <si>
+    <t>0x04B</t>
+  </si>
+  <si>
+    <t>0x04C</t>
+  </si>
+  <si>
+    <t>0x04D</t>
+  </si>
+  <si>
+    <t>0x04E</t>
+  </si>
+  <si>
+    <t>0x04F</t>
+  </si>
+  <si>
+    <t>0x05A</t>
+  </si>
+  <si>
+    <t>MOV R3, #C ROR 0</t>
   </si>
 </sst>
 </file>
@@ -876,11 +999,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E17FB6-AC76-4C3E-BEFA-6AB3607784FD}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Y93"/>
+  <dimension ref="A1:AK145"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B57" sqref="B57"/>
+      <pane ySplit="8" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K98" sqref="K98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1945,7 +2068,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="3" t="str">
-        <f t="shared" ref="S20:S22" si="1">DEC2HEX(C20*2^15 + D20*2^14 + E20*2^13 + F20*2^12 + G20*2^11 + H20*2^10 + I20*2^9 + J20*2^8 + K20*2^7 + L20*2^6 + M20*2^5 + N20*2^4 + O20 * 2 ^ 3 + P20  * 2^2 + Q20 * 2 + R20)</f>
+        <f t="shared" ref="S20:S21" si="1">DEC2HEX(C20*2^15 + D20*2^14 + E20*2^13 + F20*2^12 + G20*2^11 + H20*2^10 + I20*2^9 + J20*2^8 + K20*2^7 + L20*2^6 + M20*2^5 + N20*2^4 + O20 * 2 ^ 3 + P20  * 2^2 + Q20 * 2 + R20)</f>
         <v>1BC0</v>
       </c>
       <c r="T20" t="s">
@@ -2071,7 +2194,7 @@
         <v>0</v>
       </c>
       <c r="S22" s="3" t="str">
-        <f>DEC2HEX(C22*2^15 + D22*2^14 + E22*2^13 + F22*2^12 + G22*2^11 + H22*2^10 + I22*2^9 + J22*2^8 + K22*2^7 + L22*2^6 + M22*2^5 + N22*2^4 + O22 * 2 ^ 3 + P22  * 2^2 + Q22 * 2 + R22)</f>
+        <f t="shared" ref="S22:S28" si="2">DEC2HEX(C22*2^15 + D22*2^14 + E22*2^13 + F22*2^12 + G22*2^11 + H22*2^10 + I22*2^9 + J22*2^8 + K22*2^7 + L22*2^6 + M22*2^5 + N22*2^4 + O22 * 2 ^ 3 + P22  * 2^2 + Q22 * 2 + R22)</f>
         <v>1B00</v>
       </c>
       <c r="T22" t="s">
@@ -2134,7 +2257,7 @@
         <v>0</v>
       </c>
       <c r="S23" s="3" t="str">
-        <f>DEC2HEX(C23*2^15 + D23*2^14 + E23*2^13 + F23*2^12 + G23*2^11 + H23*2^10 + I23*2^9 + J23*2^8 + K23*2^7 + L23*2^6 + M23*2^5 + N23*2^4 + O23 * 2 ^ 3 + P23  * 2^2 + Q23 * 2 + R23)</f>
+        <f t="shared" si="2"/>
         <v>1B80</v>
       </c>
       <c r="T23" t="s">
@@ -2197,7 +2320,7 @@
         <v>1</v>
       </c>
       <c r="S24" s="3" t="str">
-        <f>DEC2HEX(C24*2^15 + D24*2^14 + E24*2^13 + F24*2^12 + G24*2^11 + H24*2^10 + I24*2^9 + J24*2^8 + K24*2^7 + L24*2^6 + M24*2^5 + N24*2^4 + O24 * 2 ^ 3 + P24  * 2^2 + Q24 * 2 + R24)</f>
+        <f t="shared" si="2"/>
         <v>1523</v>
       </c>
       <c r="T24" t="s">
@@ -2260,7 +2383,7 @@
         <v>0</v>
       </c>
       <c r="S25" s="3" t="str">
-        <f>DEC2HEX(C25*2^15 + D25*2^14 + E25*2^13 + F25*2^12 + G25*2^11 + H25*2^10 + I25*2^9 + J25*2^8 + K25*2^7 + L25*2^6 + M25*2^5 + N25*2^4 + O25 * 2 ^ 3 + P25  * 2^2 + Q25 * 2 + R25)</f>
+        <f t="shared" si="2"/>
         <v>1300</v>
       </c>
     </row>
@@ -2320,7 +2443,7 @@
         <v>0</v>
       </c>
       <c r="S26" s="3" t="str">
-        <f>DEC2HEX(C26*2^15 + D26*2^14 + E26*2^13 + F26*2^12 + G26*2^11 + H26*2^10 + I26*2^9 + J26*2^8 + K26*2^7 + L26*2^6 + M26*2^5 + N26*2^4 + O26 * 2 ^ 3 + P26  * 2^2 + Q26 * 2 + R26)</f>
+        <f t="shared" si="2"/>
         <v>CE04</v>
       </c>
     </row>
@@ -2380,7 +2503,7 @@
         <v>1</v>
       </c>
       <c r="S27" s="3" t="str">
-        <f>DEC2HEX(C27*2^15 + D27*2^14 + E27*2^13 + F27*2^12 + G27*2^11 + H27*2^10 + I27*2^9 + J27*2^8 + K27*2^7 + L27*2^6 + M27*2^5 + N27*2^4 + O27 * 2 ^ 3 + P27  * 2^2 + Q27 * 2 + R27)</f>
+        <f t="shared" si="2"/>
         <v>147</v>
       </c>
     </row>
@@ -2440,7 +2563,7 @@
         <v>1</v>
       </c>
       <c r="S28" s="3" t="str">
-        <f>DEC2HEX(C28*2^15 + D28*2^14 + E28*2^13 + F28*2^12 + G28*2^11 + H28*2^10 + I28*2^9 + J28*2^8 + K28*2^7 + L28*2^6 + M28*2^5 + N28*2^4 + O28 * 2 ^ 3 + P28  * 2^2 + Q28 * 2 + R28)</f>
+        <f t="shared" si="2"/>
         <v>403</v>
       </c>
     </row>
@@ -2500,7 +2623,7 @@
         <v>0</v>
       </c>
       <c r="S29" s="3" t="str">
-        <f t="shared" ref="S29:S62" si="2">DEC2HEX(C29*2^15 + D29*2^14 + E29*2^13 + F29*2^12 + G29*2^11 + H29*2^10 + I29*2^9 + J29*2^8 + K29*2^7 + L29*2^6 + M29*2^5 + N29*2^4 + O29 * 2 ^ 3 + P29  * 2^2 + Q29 * 2 + R29)</f>
+        <f t="shared" ref="S29:S54" si="3">DEC2HEX(C29*2^15 + D29*2^14 + E29*2^13 + F29*2^12 + G29*2^11 + H29*2^10 + I29*2^9 + J29*2^8 + K29*2^7 + L29*2^6 + M29*2^5 + N29*2^4 + O29 * 2 ^ 3 + P29  * 2^2 + Q29 * 2 + R29)</f>
         <v>CE00</v>
       </c>
     </row>
@@ -2560,7 +2683,7 @@
         <v>1</v>
       </c>
       <c r="S30" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>347</v>
       </c>
       <c r="T30" t="s">
@@ -2623,7 +2746,7 @@
         <v>0</v>
       </c>
       <c r="S31" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1380</v>
       </c>
       <c r="T31" t="s">
@@ -2686,7 +2809,7 @@
         <v>1</v>
       </c>
       <c r="S32" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>747</v>
       </c>
       <c r="T32" t="s">
@@ -2749,7 +2872,7 @@
         <v>0</v>
       </c>
       <c r="S33" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>CE06</v>
       </c>
     </row>
@@ -2809,7 +2932,7 @@
         <v>1</v>
       </c>
       <c r="S34" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>B47</v>
       </c>
       <c r="T34" t="s">
@@ -2872,7 +2995,7 @@
         <v>0</v>
       </c>
       <c r="S35" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1BC0</v>
       </c>
       <c r="T35" t="s">
@@ -2935,7 +3058,7 @@
         <v>1</v>
       </c>
       <c r="S36" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>E03</v>
       </c>
       <c r="T36" t="s">
@@ -2998,7 +3121,7 @@
         <v>1</v>
       </c>
       <c r="S37" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1E21</v>
       </c>
       <c r="T37" t="s">
@@ -3061,7 +3184,7 @@
         <v>0</v>
       </c>
       <c r="S38" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1B00</v>
       </c>
       <c r="T38" t="s">
@@ -3124,7 +3247,7 @@
         <v>0</v>
       </c>
       <c r="S39" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1BC0</v>
       </c>
       <c r="T39" t="s">
@@ -3187,7 +3310,7 @@
         <v>1</v>
       </c>
       <c r="S40" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1E21</v>
       </c>
       <c r="T40" t="s">
@@ -3250,7 +3373,7 @@
         <v>0</v>
       </c>
       <c r="S41" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1B00</v>
       </c>
       <c r="T41" t="s">
@@ -3313,7 +3436,7 @@
         <v>0</v>
       </c>
       <c r="S42" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1BC0</v>
       </c>
       <c r="T42" t="s">
@@ -3376,7 +3499,7 @@
         <v>1</v>
       </c>
       <c r="S43" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1E21</v>
       </c>
       <c r="T43" t="s">
@@ -3439,7 +3562,7 @@
         <v>0</v>
       </c>
       <c r="S44" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1B00</v>
       </c>
       <c r="T44" t="s">
@@ -3502,7 +3625,7 @@
         <v>0</v>
       </c>
       <c r="S45" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1BC0</v>
       </c>
       <c r="T45" t="s">
@@ -3565,7 +3688,7 @@
         <v>1</v>
       </c>
       <c r="S46" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1E21</v>
       </c>
       <c r="T46" t="s">
@@ -3628,7 +3751,7 @@
         <v>0</v>
       </c>
       <c r="S47" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1B00</v>
       </c>
       <c r="T47" t="s">
@@ -3691,14 +3814,14 @@
         <v>0</v>
       </c>
       <c r="S48" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1BC0</v>
       </c>
       <c r="T48" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>121</v>
       </c>
@@ -3754,14 +3877,14 @@
         <v>1</v>
       </c>
       <c r="S49" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1E21</v>
       </c>
       <c r="T49" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>122</v>
       </c>
@@ -3817,14 +3940,14 @@
         <v>0</v>
       </c>
       <c r="S50" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1B00</v>
       </c>
       <c r="T50" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>123</v>
       </c>
@@ -3884,7 +4007,7 @@
         <v>C604</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>124</v>
       </c>
@@ -3944,7 +4067,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>125</v>
       </c>
@@ -4004,7 +4127,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>126</v>
       </c>
@@ -4060,14 +4183,14 @@
         <v>0</v>
       </c>
       <c r="S54" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13C0</v>
       </c>
       <c r="T54" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>127</v>
       </c>
@@ -4123,11 +4246,11 @@
         <v>0</v>
       </c>
       <c r="S55" s="3" t="str">
-        <f>DEC2HEX(C55*2^15 + D55*2^14 + E55*2^13 + F55*2^12 + G55*2^11 + H55*2^10 + I55*2^9 + J55*2^8 + K55*2^7 + L55*2^6 + M55*2^5 + N55*2^4 + O55 * 2 ^ 3 + P55  * 2^2 + Q55 * 2 + R55)</f>
+        <f t="shared" ref="S55:S85" si="4">DEC2HEX(C55*2^15 + D55*2^14 + E55*2^13 + F55*2^12 + G55*2^11 + H55*2^10 + I55*2^9 + J55*2^8 + K55*2^7 + L55*2^6 + M55*2^5 + N55*2^4 + O55 * 2 ^ 3 + P55  * 2^2 + Q55 * 2 + R55)</f>
         <v>1B80</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>128</v>
       </c>
@@ -4183,11 +4306,11 @@
         <v>1</v>
       </c>
       <c r="S56" s="3" t="str">
-        <f>DEC2HEX(C56*2^15 + D56*2^14 + E56*2^13 + F56*2^12 + G56*2^11 + H56*2^10 + I56*2^9 + J56*2^8 + K56*2^7 + L56*2^6 + M56*2^5 + N56*2^4 + O56 * 2 ^ 3 + P56  * 2^2 + Q56 * 2 + R56)</f>
+        <f t="shared" si="4"/>
         <v>1423</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>138</v>
       </c>
@@ -4243,11 +4366,11 @@
         <v>0</v>
       </c>
       <c r="S57" s="3" t="str">
-        <f>DEC2HEX(C57*2^15 + D57*2^14 + E57*2^13 + F57*2^12 + G57*2^11 + H57*2^10 + I57*2^9 + J57*2^8 + K57*2^7 + L57*2^6 + M57*2^5 + N57*2^4 + O57 * 2 ^ 3 + P57  * 2^2 + Q57 * 2 + R57)</f>
+        <f t="shared" si="4"/>
         <v>1300</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>140</v>
       </c>
@@ -4303,11 +4426,11 @@
         <v>0</v>
       </c>
       <c r="S58" s="3" t="str">
-        <f>DEC2HEX(C58*2^15 + D58*2^14 + E58*2^13 + F58*2^12 + G58*2^11 + H58*2^10 + I58*2^9 + J58*2^8 + K58*2^7 + L58*2^6 + M58*2^5 + N58*2^4 + O58 * 2 ^ 3 + P58  * 2^2 + Q58 * 2 + R58)</f>
+        <f t="shared" si="4"/>
         <v>CE08</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>139</v>
       </c>
@@ -4363,11 +4486,11 @@
         <v>1</v>
       </c>
       <c r="S59" s="3" t="str">
-        <f>DEC2HEX(C59*2^15 + D59*2^14 + E59*2^13 + F59*2^12 + G59*2^11 + H59*2^10 + I59*2^9 + J59*2^8 + K59*2^7 + L59*2^6 + M59*2^5 + N59*2^4 + O59 * 2 ^ 3 + P59  * 2^2 + Q59 * 2 + R59)</f>
+        <f t="shared" si="4"/>
         <v>147</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>144</v>
       </c>
@@ -4423,37 +4546,37 @@
         <v>1</v>
       </c>
       <c r="S60" s="3" t="str">
-        <f>DEC2HEX(C60*2^15 + D60*2^14 + E60*2^13 + F60*2^12 + G60*2^11 + H60*2^10 + I60*2^9 + J60*2^8 + K60*2^7 + L60*2^6 + M60*2^5 + N60*2^4 + O60 * 2 ^ 3 + P60  * 2^2 + Q60 * 2 + R60)</f>
+        <f t="shared" si="4"/>
         <v>403</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>145</v>
       </c>
       <c r="B61" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D61">
         <v>1</v>
       </c>
       <c r="E61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J61">
         <v>0</v>
@@ -4483,65 +4606,818 @@
         <v>0</v>
       </c>
       <c r="S61" s="3" t="str">
-        <f>DEC2HEX(C61*2^15 + D61*2^14 + E61*2^13 + F61*2^12 + G61*2^11 + H61*2^10 + I61*2^9 + J61*2^8 + K61*2^7 + L61*2^6 + M61*2^5 + N61*2^4 + O61 * 2 ^ 3 + P61  * 2^2 + Q61 * 2 + R61)</f>
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="S63" s="3"/>
-    </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B64" s="5"/>
-      <c r="S64" s="3"/>
+        <f t="shared" si="4"/>
+        <v>CE00</v>
+      </c>
+      <c r="AK61" s="3"/>
+    </row>
+    <row r="62" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>148</v>
+      </c>
+      <c r="B62" t="s">
+        <v>83</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62">
+        <v>1</v>
+      </c>
+      <c r="J62">
+        <v>1</v>
+      </c>
+      <c r="K62">
+        <v>0</v>
+      </c>
+      <c r="L62">
+        <v>1</v>
+      </c>
+      <c r="M62">
+        <v>0</v>
+      </c>
+      <c r="N62">
+        <v>0</v>
+      </c>
+      <c r="O62">
+        <v>0</v>
+      </c>
+      <c r="P62">
+        <v>1</v>
+      </c>
+      <c r="Q62">
+        <v>1</v>
+      </c>
+      <c r="R62">
+        <v>1</v>
+      </c>
+      <c r="S62" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>347</v>
+      </c>
+    </row>
+    <row r="63" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>149</v>
+      </c>
+      <c r="B63" t="s">
+        <v>129</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>1</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63">
+        <v>1</v>
+      </c>
+      <c r="J63">
+        <v>1</v>
+      </c>
+      <c r="K63">
+        <v>1</v>
+      </c>
+      <c r="L63">
+        <v>0</v>
+      </c>
+      <c r="M63">
+        <v>0</v>
+      </c>
+      <c r="N63">
+        <v>0</v>
+      </c>
+      <c r="O63">
+        <v>0</v>
+      </c>
+      <c r="P63">
+        <v>0</v>
+      </c>
+      <c r="Q63">
+        <v>0</v>
+      </c>
+      <c r="R63">
+        <v>0</v>
+      </c>
+      <c r="S63" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="64" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>150</v>
+      </c>
+      <c r="B64" t="s">
+        <v>84</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="H64">
+        <v>1</v>
+      </c>
+      <c r="I64">
+        <v>1</v>
+      </c>
+      <c r="J64">
+        <v>1</v>
+      </c>
+      <c r="K64">
+        <v>0</v>
+      </c>
+      <c r="L64">
+        <v>1</v>
+      </c>
+      <c r="M64">
+        <v>0</v>
+      </c>
+      <c r="N64">
+        <v>0</v>
+      </c>
+      <c r="O64">
+        <v>0</v>
+      </c>
+      <c r="P64">
+        <v>1</v>
+      </c>
+      <c r="Q64">
+        <v>1</v>
+      </c>
+      <c r="R64">
+        <v>1</v>
+      </c>
+      <c r="S64" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>747</v>
+      </c>
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="S65" s="3"/>
+      <c r="A65" t="s">
+        <v>151</v>
+      </c>
+      <c r="B65" t="s">
+        <v>146</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>1</v>
+      </c>
+      <c r="H65">
+        <v>1</v>
+      </c>
+      <c r="I65">
+        <v>1</v>
+      </c>
+      <c r="J65">
+        <v>0</v>
+      </c>
+      <c r="K65">
+        <v>0</v>
+      </c>
+      <c r="L65">
+        <v>0</v>
+      </c>
+      <c r="M65">
+        <v>0</v>
+      </c>
+      <c r="N65">
+        <v>0</v>
+      </c>
+      <c r="O65">
+        <v>1</v>
+      </c>
+      <c r="P65">
+        <v>0</v>
+      </c>
+      <c r="Q65">
+        <v>1</v>
+      </c>
+      <c r="R65">
+        <v>0</v>
+      </c>
+      <c r="S65" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>CE0A</v>
+      </c>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="S66" s="3"/>
+      <c r="A66" t="s">
+        <v>152</v>
+      </c>
+      <c r="B66" t="s">
+        <v>87</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <v>1</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+      <c r="I66">
+        <v>1</v>
+      </c>
+      <c r="J66">
+        <v>1</v>
+      </c>
+      <c r="K66">
+        <v>0</v>
+      </c>
+      <c r="L66">
+        <v>1</v>
+      </c>
+      <c r="M66">
+        <v>0</v>
+      </c>
+      <c r="N66">
+        <v>0</v>
+      </c>
+      <c r="O66">
+        <v>0</v>
+      </c>
+      <c r="P66">
+        <v>1</v>
+      </c>
+      <c r="Q66">
+        <v>1</v>
+      </c>
+      <c r="R66">
+        <v>1</v>
+      </c>
+      <c r="S66" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>B47</v>
+      </c>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="S67" s="3"/>
+      <c r="A67" t="s">
+        <v>173</v>
+      </c>
+      <c r="B67" t="s">
+        <v>130</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>1</v>
+      </c>
+      <c r="G67">
+        <v>1</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+      <c r="I67">
+        <v>1</v>
+      </c>
+      <c r="J67">
+        <v>1</v>
+      </c>
+      <c r="K67">
+        <v>1</v>
+      </c>
+      <c r="L67">
+        <v>1</v>
+      </c>
+      <c r="M67">
+        <v>0</v>
+      </c>
+      <c r="N67">
+        <v>0</v>
+      </c>
+      <c r="O67">
+        <v>0</v>
+      </c>
+      <c r="P67">
+        <v>0</v>
+      </c>
+      <c r="Q67">
+        <v>0</v>
+      </c>
+      <c r="R67">
+        <v>0</v>
+      </c>
+      <c r="S67" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>1BC0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>174</v>
+      </c>
+      <c r="B68" t="s">
+        <v>89</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
+      </c>
+      <c r="H68">
+        <v>1</v>
+      </c>
+      <c r="I68">
+        <v>1</v>
+      </c>
+      <c r="J68">
+        <v>0</v>
+      </c>
+      <c r="K68">
+        <v>0</v>
+      </c>
+      <c r="L68">
+        <v>0</v>
+      </c>
+      <c r="M68">
+        <v>0</v>
+      </c>
+      <c r="N68">
+        <v>0</v>
+      </c>
+      <c r="O68">
+        <v>0</v>
+      </c>
+      <c r="P68">
+        <v>0</v>
+      </c>
+      <c r="Q68">
+        <v>1</v>
+      </c>
+      <c r="R68">
+        <v>1</v>
+      </c>
+      <c r="S68" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>E03</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>175</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>1</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
+      </c>
+      <c r="H69">
+        <v>1</v>
+      </c>
+      <c r="I69">
+        <v>1</v>
+      </c>
+      <c r="J69">
+        <v>0</v>
+      </c>
+      <c r="K69">
+        <v>0</v>
+      </c>
+      <c r="L69">
+        <v>0</v>
+      </c>
+      <c r="M69">
+        <v>1</v>
+      </c>
+      <c r="N69">
+        <v>0</v>
+      </c>
+      <c r="O69">
+        <v>0</v>
+      </c>
+      <c r="P69">
+        <v>0</v>
+      </c>
+      <c r="Q69">
+        <v>0</v>
+      </c>
+      <c r="R69">
+        <v>1</v>
+      </c>
+      <c r="S69" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>1E21</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>176</v>
+      </c>
+      <c r="B70" t="s">
+        <v>95</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>1</v>
+      </c>
+      <c r="G70">
+        <v>1</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+      <c r="I70">
+        <v>1</v>
+      </c>
+      <c r="J70">
+        <v>1</v>
+      </c>
+      <c r="K70">
+        <v>0</v>
+      </c>
+      <c r="L70">
+        <v>0</v>
+      </c>
+      <c r="M70">
+        <v>0</v>
+      </c>
+      <c r="N70">
+        <v>0</v>
+      </c>
+      <c r="O70">
+        <v>0</v>
+      </c>
+      <c r="P70">
+        <v>0</v>
+      </c>
+      <c r="Q70">
+        <v>0</v>
+      </c>
+      <c r="R70">
+        <v>0</v>
+      </c>
+      <c r="S70" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>1B00</v>
+      </c>
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="S71" s="3"/>
+      <c r="A71" t="s">
+        <v>177</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>1</v>
+      </c>
+      <c r="G71">
+        <v>1</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+      <c r="I71">
+        <v>1</v>
+      </c>
+      <c r="J71">
+        <v>1</v>
+      </c>
+      <c r="K71">
+        <v>1</v>
+      </c>
+      <c r="L71">
+        <v>1</v>
+      </c>
+      <c r="M71">
+        <v>0</v>
+      </c>
+      <c r="N71">
+        <v>0</v>
+      </c>
+      <c r="O71">
+        <v>0</v>
+      </c>
+      <c r="P71">
+        <v>0</v>
+      </c>
+      <c r="Q71">
+        <v>0</v>
+      </c>
+      <c r="R71">
+        <v>0</v>
+      </c>
+      <c r="S71" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>1BC0</v>
+      </c>
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="S72" s="3"/>
+      <c r="A72" t="s">
+        <v>178</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>1</v>
+      </c>
+      <c r="G72">
+        <v>1</v>
+      </c>
+      <c r="H72">
+        <v>1</v>
+      </c>
+      <c r="I72">
+        <v>1</v>
+      </c>
+      <c r="J72">
+        <v>0</v>
+      </c>
+      <c r="K72">
+        <v>0</v>
+      </c>
+      <c r="L72">
+        <v>0</v>
+      </c>
+      <c r="M72">
+        <v>1</v>
+      </c>
+      <c r="N72">
+        <v>0</v>
+      </c>
+      <c r="O72">
+        <v>0</v>
+      </c>
+      <c r="P72">
+        <v>0</v>
+      </c>
+      <c r="Q72">
+        <v>0</v>
+      </c>
+      <c r="R72">
+        <v>1</v>
+      </c>
+      <c r="S72" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>1E21</v>
+      </c>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="S73" s="3"/>
+      <c r="A73" t="s">
+        <v>153</v>
+      </c>
+      <c r="B73" t="s">
+        <v>95</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <v>1</v>
+      </c>
+      <c r="G73">
+        <v>1</v>
+      </c>
+      <c r="H73">
+        <v>0</v>
+      </c>
+      <c r="I73">
+        <v>1</v>
+      </c>
+      <c r="J73">
+        <v>1</v>
+      </c>
+      <c r="K73">
+        <v>0</v>
+      </c>
+      <c r="L73">
+        <v>0</v>
+      </c>
+      <c r="M73">
+        <v>0</v>
+      </c>
+      <c r="N73">
+        <v>0</v>
+      </c>
+      <c r="O73">
+        <v>0</v>
+      </c>
+      <c r="P73">
+        <v>0</v>
+      </c>
+      <c r="Q73">
+        <v>0</v>
+      </c>
+      <c r="R73">
+        <v>0</v>
+      </c>
+      <c r="S73" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>1B00</v>
+      </c>
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="S74" s="3"/>
+      <c r="A74" t="s">
+        <v>154</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <v>1</v>
+      </c>
+      <c r="G74">
+        <v>1</v>
+      </c>
+      <c r="H74">
+        <v>0</v>
+      </c>
+      <c r="I74">
+        <v>1</v>
+      </c>
+      <c r="J74">
+        <v>1</v>
+      </c>
+      <c r="K74">
+        <v>1</v>
+      </c>
+      <c r="L74">
+        <v>1</v>
+      </c>
+      <c r="M74">
+        <v>0</v>
+      </c>
+      <c r="N74">
+        <v>0</v>
+      </c>
+      <c r="O74">
+        <v>0</v>
+      </c>
+      <c r="P74">
+        <v>0</v>
+      </c>
+      <c r="Q74">
+        <v>0</v>
+      </c>
+      <c r="R74">
+        <v>0</v>
+      </c>
+      <c r="S74" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>1BC0</v>
+      </c>
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A75" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="B75" t="s">
-        <v>45</v>
+      <c r="A75" t="s">
+        <v>155</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>94</v>
       </c>
       <c r="C75">
         <v>0</v>
       </c>
       <c r="D75">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E75">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F75">
         <v>1</v>
       </c>
       <c r="G75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J75">
         <v>0</v>
@@ -4553,7 +5429,7 @@
         <v>0</v>
       </c>
       <c r="M75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N75">
         <v>0</v>
@@ -4568,79 +5444,79 @@
         <v>0</v>
       </c>
       <c r="R75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S75" s="3" t="str">
-        <f>DEC2HEX(C75*2^15 + D75*2^14 + E75*2^13 + F75*2^12 + G75*2^11 + H75*2^10 + I75*2^9 + J75*2^8 + K75*2^7 + L75*2^6 + M75*2^5 + N75*2^4 + O75 * 2 ^ 3 + P75  * 2^2 + Q75 * 2 + R75)</f>
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="76" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>1E21</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>23</v>
-      </c>
-      <c r="B76" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="C76" s="6">
-        <v>0</v>
-      </c>
-      <c r="D76" s="7">
-        <v>0</v>
-      </c>
-      <c r="E76" s="7">
-        <v>0</v>
-      </c>
-      <c r="F76" s="7">
-        <v>0</v>
-      </c>
-      <c r="G76" s="7">
-        <v>1</v>
-      </c>
-      <c r="H76" s="7">
-        <v>1</v>
-      </c>
-      <c r="I76" s="7">
-        <v>1</v>
-      </c>
-      <c r="J76" s="7">
-        <v>1</v>
-      </c>
-      <c r="K76" s="7">
-        <v>1</v>
-      </c>
-      <c r="L76" s="7">
-        <v>1</v>
-      </c>
-      <c r="M76" s="7">
-        <v>0</v>
-      </c>
-      <c r="N76" s="7">
-        <v>1</v>
-      </c>
-      <c r="O76" s="7">
-        <v>1</v>
-      </c>
-      <c r="P76" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q76" s="7">
-        <v>1</v>
-      </c>
-      <c r="R76" s="7">
-        <v>1</v>
+        <v>156</v>
+      </c>
+      <c r="B76" t="s">
+        <v>95</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="F76">
+        <v>1</v>
+      </c>
+      <c r="G76">
+        <v>1</v>
+      </c>
+      <c r="H76">
+        <v>0</v>
+      </c>
+      <c r="I76">
+        <v>1</v>
+      </c>
+      <c r="J76">
+        <v>1</v>
+      </c>
+      <c r="K76">
+        <v>0</v>
+      </c>
+      <c r="L76">
+        <v>0</v>
+      </c>
+      <c r="M76">
+        <v>0</v>
+      </c>
+      <c r="N76">
+        <v>0</v>
+      </c>
+      <c r="O76">
+        <v>0</v>
+      </c>
+      <c r="P76">
+        <v>0</v>
+      </c>
+      <c r="Q76">
+        <v>0</v>
+      </c>
+      <c r="R76">
+        <v>0</v>
       </c>
       <c r="S76" s="3" t="str">
-        <f>DEC2HEX(C76*2^15 + D76*2^14 + E76*2^13 + F76*2^12 + G76*2^11 + H76*2^10 + I76*2^9 + J76*2^8 + K76*2^7 + L76*2^6 + M76*2^5 + N76*2^4 + O76 * 2 ^ 3 + P76  * 2^2 + Q76 * 2 + R76)</f>
-        <v>FDB</v>
-      </c>
-    </row>
-    <row r="77" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>1B00</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>24</v>
-      </c>
-      <c r="B77" s="14" t="s">
-        <v>61</v>
+        <v>157</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>130</v>
       </c>
       <c r="C77">
         <v>0</v>
@@ -4649,7 +5525,7 @@
         <v>0</v>
       </c>
       <c r="E77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F77">
         <v>1</v>
@@ -4658,7 +5534,7 @@
         <v>1</v>
       </c>
       <c r="H77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I77">
         <v>1</v>
@@ -4679,7 +5555,7 @@
         <v>0</v>
       </c>
       <c r="O77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P77">
         <v>0</v>
@@ -4688,564 +5564,2149 @@
         <v>0</v>
       </c>
       <c r="R77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S77" s="3" t="str">
-        <f t="shared" ref="S77:S79" si="3">DEC2HEX(C77*2^15 + D77*2^14 + E77*2^13 + F77*2^12 + G77*2^11 + H77*2^10 + I77*2^9 + J77*2^8 + K77*2^7 + L77*2^6 + M77*2^5 + N77*2^4 + O77 * 2 ^ 3 + P77  * 2^2 + Q77 * 2 + R77)</f>
-        <v>3FC9</v>
-      </c>
-    </row>
-    <row r="78" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>1BC0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>25</v>
-      </c>
-      <c r="B78" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="C78" s="7">
-        <v>1</v>
-      </c>
-      <c r="D78" s="7">
-        <v>0</v>
-      </c>
-      <c r="E78" s="7">
-        <v>1</v>
-      </c>
-      <c r="F78" s="7">
-        <v>0</v>
-      </c>
-      <c r="G78" s="7">
-        <v>1</v>
-      </c>
-      <c r="H78" s="7">
-        <v>0</v>
-      </c>
-      <c r="I78" s="7">
-        <v>1</v>
-      </c>
-      <c r="J78" s="7">
-        <v>0</v>
-      </c>
-      <c r="K78" s="7">
-        <v>1</v>
-      </c>
-      <c r="L78" s="7">
-        <v>0</v>
-      </c>
-      <c r="M78" s="7">
-        <v>1</v>
-      </c>
-      <c r="N78" s="7">
-        <v>0</v>
-      </c>
-      <c r="O78" s="7">
-        <v>1</v>
-      </c>
-      <c r="P78" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q78" s="7">
-        <v>1</v>
-      </c>
-      <c r="R78" s="7">
+        <v>158</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="F78">
+        <v>1</v>
+      </c>
+      <c r="G78">
+        <v>1</v>
+      </c>
+      <c r="H78">
+        <v>1</v>
+      </c>
+      <c r="I78">
+        <v>1</v>
+      </c>
+      <c r="J78">
+        <v>0</v>
+      </c>
+      <c r="K78">
+        <v>0</v>
+      </c>
+      <c r="L78">
+        <v>0</v>
+      </c>
+      <c r="M78">
+        <v>1</v>
+      </c>
+      <c r="N78">
+        <v>0</v>
+      </c>
+      <c r="O78">
+        <v>0</v>
+      </c>
+      <c r="P78">
+        <v>0</v>
+      </c>
+      <c r="Q78">
+        <v>0</v>
+      </c>
+      <c r="R78">
         <v>1</v>
       </c>
       <c r="S78" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>AAAB</v>
-      </c>
-    </row>
-    <row r="79" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>1E21</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>26</v>
-      </c>
-      <c r="B79" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C79" s="7">
-        <v>0</v>
-      </c>
-      <c r="D79" s="7">
-        <v>0</v>
-      </c>
-      <c r="E79" s="7">
-        <v>1</v>
-      </c>
-      <c r="F79" s="7">
-        <v>1</v>
-      </c>
-      <c r="G79" s="7">
-        <v>1</v>
-      </c>
-      <c r="H79" s="7">
-        <v>1</v>
-      </c>
-      <c r="I79" s="7">
-        <v>1</v>
-      </c>
-      <c r="J79" s="7">
-        <v>0</v>
-      </c>
-      <c r="K79" s="7">
-        <v>0</v>
-      </c>
-      <c r="L79" s="7">
-        <v>0</v>
-      </c>
-      <c r="M79" s="7">
-        <v>1</v>
-      </c>
-      <c r="N79" s="7">
-        <v>0</v>
-      </c>
-      <c r="O79" s="7">
-        <v>1</v>
-      </c>
-      <c r="P79" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q79" s="7">
-        <v>1</v>
-      </c>
-      <c r="R79" s="7">
+        <v>159</v>
+      </c>
+      <c r="B79" t="s">
+        <v>95</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="F79">
+        <v>1</v>
+      </c>
+      <c r="G79">
+        <v>1</v>
+      </c>
+      <c r="H79">
+        <v>0</v>
+      </c>
+      <c r="I79">
+        <v>1</v>
+      </c>
+      <c r="J79">
+        <v>1</v>
+      </c>
+      <c r="K79">
+        <v>0</v>
+      </c>
+      <c r="L79">
+        <v>0</v>
+      </c>
+      <c r="M79">
+        <v>0</v>
+      </c>
+      <c r="N79">
+        <v>0</v>
+      </c>
+      <c r="O79">
+        <v>0</v>
+      </c>
+      <c r="P79">
+        <v>0</v>
+      </c>
+      <c r="Q79">
+        <v>0</v>
+      </c>
+      <c r="R79">
         <v>0</v>
       </c>
       <c r="S79" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>3E2A</v>
+        <f t="shared" si="4"/>
+        <v>1B00</v>
       </c>
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>27</v>
-      </c>
-      <c r="B80" s="14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="F80">
+        <v>1</v>
+      </c>
+      <c r="G80">
+        <v>1</v>
+      </c>
+      <c r="H80">
+        <v>0</v>
+      </c>
+      <c r="I80">
+        <v>1</v>
+      </c>
+      <c r="J80">
+        <v>1</v>
+      </c>
+      <c r="K80">
+        <v>1</v>
+      </c>
+      <c r="L80">
+        <v>1</v>
+      </c>
+      <c r="M80">
+        <v>0</v>
+      </c>
+      <c r="N80">
+        <v>0</v>
+      </c>
+      <c r="O80">
+        <v>0</v>
+      </c>
+      <c r="P80">
+        <v>0</v>
+      </c>
+      <c r="Q80">
+        <v>0</v>
+      </c>
+      <c r="R80">
+        <v>0</v>
+      </c>
+      <c r="S80" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>1BC0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>28</v>
-      </c>
-      <c r="B81" s="14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="82" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+      <c r="F81">
+        <v>1</v>
+      </c>
+      <c r="G81">
+        <v>1</v>
+      </c>
+      <c r="H81">
+        <v>1</v>
+      </c>
+      <c r="I81">
+        <v>1</v>
+      </c>
+      <c r="J81">
+        <v>0</v>
+      </c>
+      <c r="K81">
+        <v>0</v>
+      </c>
+      <c r="L81">
+        <v>0</v>
+      </c>
+      <c r="M81">
+        <v>1</v>
+      </c>
+      <c r="N81">
+        <v>0</v>
+      </c>
+      <c r="O81">
+        <v>0</v>
+      </c>
+      <c r="P81">
+        <v>0</v>
+      </c>
+      <c r="Q81">
+        <v>0</v>
+      </c>
+      <c r="R81">
+        <v>1</v>
+      </c>
+      <c r="S81" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>1E21</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>29</v>
-      </c>
-      <c r="B82" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="C82" s="7">
-        <v>1</v>
-      </c>
-      <c r="D82" s="7">
-        <v>0</v>
-      </c>
-      <c r="E82" s="7">
-        <v>0</v>
-      </c>
-      <c r="F82" s="7">
-        <v>0</v>
-      </c>
-      <c r="G82" s="7">
-        <v>1</v>
-      </c>
-      <c r="H82" s="7">
-        <v>0</v>
-      </c>
-      <c r="I82" s="7">
-        <v>0</v>
-      </c>
-      <c r="J82" s="7">
-        <v>0</v>
-      </c>
-      <c r="K82" s="7">
-        <v>1</v>
-      </c>
-      <c r="L82" s="7">
-        <v>0</v>
-      </c>
-      <c r="M82" s="7">
-        <v>0</v>
-      </c>
-      <c r="N82" s="7">
-        <v>0</v>
-      </c>
-      <c r="O82" s="7">
-        <v>1</v>
-      </c>
-      <c r="P82" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q82" s="7">
-        <v>0</v>
-      </c>
-      <c r="R82" s="7">
-        <v>1</v>
+        <v>162</v>
+      </c>
+      <c r="B82" t="s">
+        <v>95</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="F82">
+        <v>1</v>
+      </c>
+      <c r="G82">
+        <v>1</v>
+      </c>
+      <c r="H82">
+        <v>0</v>
+      </c>
+      <c r="I82">
+        <v>1</v>
+      </c>
+      <c r="J82">
+        <v>1</v>
+      </c>
+      <c r="K82">
+        <v>0</v>
+      </c>
+      <c r="L82">
+        <v>0</v>
+      </c>
+      <c r="M82">
+        <v>0</v>
+      </c>
+      <c r="N82">
+        <v>0</v>
+      </c>
+      <c r="O82">
+        <v>0</v>
+      </c>
+      <c r="P82">
+        <v>0</v>
+      </c>
+      <c r="Q82">
+        <v>0</v>
+      </c>
+      <c r="R82">
+        <v>0</v>
       </c>
       <c r="S82" s="3" t="str">
-        <f t="shared" ref="S82:S83" si="4">DEC2HEX(C82*2^15 + D82*2^14 + E82*2^13 + F82*2^12 + G82*2^11 + H82*2^10 + I82*2^9 + J82*2^8 + K82*2^7 + L82*2^6 + M82*2^5 + N82*2^4 + O82 * 2 ^ 3 + P82  * 2^2 + Q82 * 2 + R82)</f>
-        <v>8889</v>
-      </c>
-    </row>
-    <row r="83" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>1B00</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>30</v>
-      </c>
-      <c r="B83" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="C83" s="7">
-        <v>0</v>
-      </c>
-      <c r="D83" s="7">
-        <v>0</v>
-      </c>
-      <c r="E83" s="7">
-        <v>1</v>
-      </c>
-      <c r="F83" s="7">
-        <v>1</v>
-      </c>
-      <c r="G83" s="7">
-        <v>1</v>
-      </c>
-      <c r="H83" s="7">
-        <v>1</v>
-      </c>
-      <c r="I83" s="7">
-        <v>0</v>
-      </c>
-      <c r="J83" s="7">
-        <v>0</v>
-      </c>
-      <c r="K83" s="7">
-        <v>0</v>
-      </c>
-      <c r="L83" s="7">
-        <v>0</v>
-      </c>
-      <c r="M83" s="7">
-        <v>0</v>
-      </c>
-      <c r="N83" s="7">
-        <v>0</v>
-      </c>
-      <c r="O83" s="7">
-        <v>1</v>
-      </c>
-      <c r="P83" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q83" s="7">
-        <v>0</v>
-      </c>
-      <c r="R83" s="7">
+        <v>179</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+      <c r="F83">
+        <v>1</v>
+      </c>
+      <c r="G83">
+        <v>1</v>
+      </c>
+      <c r="H83">
+        <v>0</v>
+      </c>
+      <c r="I83">
+        <v>1</v>
+      </c>
+      <c r="J83">
+        <v>1</v>
+      </c>
+      <c r="K83">
+        <v>1</v>
+      </c>
+      <c r="L83">
+        <v>1</v>
+      </c>
+      <c r="M83">
+        <v>0</v>
+      </c>
+      <c r="N83">
+        <v>0</v>
+      </c>
+      <c r="O83">
+        <v>0</v>
+      </c>
+      <c r="P83">
+        <v>0</v>
+      </c>
+      <c r="Q83">
+        <v>0</v>
+      </c>
+      <c r="R83">
         <v>0</v>
       </c>
       <c r="S83" s="3" t="str">
         <f t="shared" si="4"/>
+        <v>1BC0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>180</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+      <c r="F84">
+        <v>1</v>
+      </c>
+      <c r="G84">
+        <v>1</v>
+      </c>
+      <c r="H84">
+        <v>1</v>
+      </c>
+      <c r="I84">
+        <v>1</v>
+      </c>
+      <c r="J84">
+        <v>0</v>
+      </c>
+      <c r="K84">
+        <v>0</v>
+      </c>
+      <c r="L84">
+        <v>0</v>
+      </c>
+      <c r="M84">
+        <v>1</v>
+      </c>
+      <c r="N84">
+        <v>0</v>
+      </c>
+      <c r="O84">
+        <v>0</v>
+      </c>
+      <c r="P84">
+        <v>0</v>
+      </c>
+      <c r="Q84">
+        <v>0</v>
+      </c>
+      <c r="R84">
+        <v>1</v>
+      </c>
+      <c r="S84" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>1E21</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>181</v>
+      </c>
+      <c r="B85" t="s">
+        <v>95</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="F85">
+        <v>1</v>
+      </c>
+      <c r="G85">
+        <v>1</v>
+      </c>
+      <c r="H85">
+        <v>0</v>
+      </c>
+      <c r="I85">
+        <v>1</v>
+      </c>
+      <c r="J85">
+        <v>1</v>
+      </c>
+      <c r="K85">
+        <v>0</v>
+      </c>
+      <c r="L85">
+        <v>0</v>
+      </c>
+      <c r="M85">
+        <v>0</v>
+      </c>
+      <c r="N85">
+        <v>0</v>
+      </c>
+      <c r="O85">
+        <v>0</v>
+      </c>
+      <c r="P85">
+        <v>0</v>
+      </c>
+      <c r="Q85">
+        <v>0</v>
+      </c>
+      <c r="R85">
+        <v>0</v>
+      </c>
+      <c r="S85" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>1B00</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>182</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+      <c r="E86">
+        <v>0</v>
+      </c>
+      <c r="F86">
+        <v>1</v>
+      </c>
+      <c r="G86">
+        <v>1</v>
+      </c>
+      <c r="H86">
+        <v>0</v>
+      </c>
+      <c r="I86">
+        <v>1</v>
+      </c>
+      <c r="J86">
+        <v>1</v>
+      </c>
+      <c r="K86">
+        <v>1</v>
+      </c>
+      <c r="L86">
+        <v>1</v>
+      </c>
+      <c r="M86">
+        <v>0</v>
+      </c>
+      <c r="N86">
+        <v>0</v>
+      </c>
+      <c r="O86">
+        <v>0</v>
+      </c>
+      <c r="P86">
+        <v>0</v>
+      </c>
+      <c r="Q86">
+        <v>0</v>
+      </c>
+      <c r="R86">
+        <v>0</v>
+      </c>
+      <c r="S86" s="3" t="str">
+        <f t="shared" ref="S86:S88" si="5">DEC2HEX(C86*2^15 + D86*2^14 + E86*2^13 + F86*2^12 + G86*2^11 + H86*2^10 + I86*2^9 + J86*2^8 + K86*2^7 + L86*2^6 + M86*2^5 + N86*2^4 + O86 * 2 ^ 3 + P86  * 2^2 + Q86 * 2 + R86)</f>
+        <v>1BC0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>183</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87">
+        <v>0</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
+      <c r="F87">
+        <v>1</v>
+      </c>
+      <c r="G87">
+        <v>1</v>
+      </c>
+      <c r="H87">
+        <v>1</v>
+      </c>
+      <c r="I87">
+        <v>1</v>
+      </c>
+      <c r="J87">
+        <v>0</v>
+      </c>
+      <c r="K87">
+        <v>0</v>
+      </c>
+      <c r="L87">
+        <v>0</v>
+      </c>
+      <c r="M87">
+        <v>1</v>
+      </c>
+      <c r="N87">
+        <v>0</v>
+      </c>
+      <c r="O87">
+        <v>0</v>
+      </c>
+      <c r="P87">
+        <v>0</v>
+      </c>
+      <c r="Q87">
+        <v>0</v>
+      </c>
+      <c r="R87">
+        <v>1</v>
+      </c>
+      <c r="S87" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>1E21</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>184</v>
+      </c>
+      <c r="B88" t="s">
+        <v>95</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="E88">
+        <v>0</v>
+      </c>
+      <c r="F88">
+        <v>1</v>
+      </c>
+      <c r="G88">
+        <v>1</v>
+      </c>
+      <c r="H88">
+        <v>0</v>
+      </c>
+      <c r="I88">
+        <v>1</v>
+      </c>
+      <c r="J88">
+        <v>1</v>
+      </c>
+      <c r="K88">
+        <v>0</v>
+      </c>
+      <c r="L88">
+        <v>0</v>
+      </c>
+      <c r="M88">
+        <v>0</v>
+      </c>
+      <c r="N88">
+        <v>0</v>
+      </c>
+      <c r="O88">
+        <v>0</v>
+      </c>
+      <c r="P88">
+        <v>0</v>
+      </c>
+      <c r="Q88">
+        <v>0</v>
+      </c>
+      <c r="R88">
+        <v>0</v>
+      </c>
+      <c r="S88" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>1B00</v>
+      </c>
+    </row>
+    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>163</v>
+      </c>
+      <c r="B89" t="s">
+        <v>147</v>
+      </c>
+      <c r="C89">
+        <v>1</v>
+      </c>
+      <c r="D89">
+        <v>1</v>
+      </c>
+      <c r="E89">
+        <v>0</v>
+      </c>
+      <c r="F89">
+        <v>0</v>
+      </c>
+      <c r="G89">
+        <v>0</v>
+      </c>
+      <c r="H89">
+        <v>1</v>
+      </c>
+      <c r="I89">
+        <v>1</v>
+      </c>
+      <c r="J89">
+        <v>0</v>
+      </c>
+      <c r="K89">
+        <v>0</v>
+      </c>
+      <c r="L89">
+        <v>0</v>
+      </c>
+      <c r="M89">
+        <v>0</v>
+      </c>
+      <c r="N89">
+        <v>0</v>
+      </c>
+      <c r="O89">
+        <v>1</v>
+      </c>
+      <c r="P89">
+        <v>0</v>
+      </c>
+      <c r="Q89">
+        <v>0</v>
+      </c>
+      <c r="R89">
+        <v>0</v>
+      </c>
+      <c r="S89" s="3" t="str">
+        <f>DEC2HEX(C89*2^15 + D89*2^14 + E89*2^13 + F89*2^12 + G89*2^11 + H89*2^10 + I89*2^9 + J89*2^8 + K89*2^7 + L89*2^6 + M89*2^5 + N89*2^4 + O89 * 2 ^ 3 + P89  * 2^2 + Q89 * 2 + R89)</f>
+        <v>C608</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>164</v>
+      </c>
+      <c r="B90" t="s">
+        <v>142</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+      <c r="E90">
+        <v>0</v>
+      </c>
+      <c r="F90">
+        <v>0</v>
+      </c>
+      <c r="G90">
+        <v>0</v>
+      </c>
+      <c r="H90">
+        <v>0</v>
+      </c>
+      <c r="I90">
+        <v>1</v>
+      </c>
+      <c r="J90">
+        <v>1</v>
+      </c>
+      <c r="K90">
+        <v>0</v>
+      </c>
+      <c r="L90">
+        <v>1</v>
+      </c>
+      <c r="M90">
+        <v>0</v>
+      </c>
+      <c r="N90">
+        <v>0</v>
+      </c>
+      <c r="O90">
+        <v>0</v>
+      </c>
+      <c r="P90">
+        <v>1</v>
+      </c>
+      <c r="Q90">
+        <v>0</v>
+      </c>
+      <c r="R90">
+        <v>1</v>
+      </c>
+      <c r="S90" s="3" t="str">
+        <f>DEC2HEX(C90*2^15 + D90*2^14 + E90*2^13 + F90*2^12 + G90*2^11 + H90*2^10 + I90*2^9 + J90*2^8 + K90*2^7 + L90*2^6 + M90*2^5 + N90*2^4 + O90 * 2 ^ 3 + P90  * 2^2 + Q90 * 2 + R90)</f>
+        <v>345</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>165</v>
+      </c>
+      <c r="B91" t="s">
+        <v>143</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+      <c r="D91">
+        <v>0</v>
+      </c>
+      <c r="E91">
+        <v>0</v>
+      </c>
+      <c r="F91">
+        <v>0</v>
+      </c>
+      <c r="G91">
+        <v>0</v>
+      </c>
+      <c r="H91">
+        <v>1</v>
+      </c>
+      <c r="I91">
+        <v>1</v>
+      </c>
+      <c r="J91">
+        <v>0</v>
+      </c>
+      <c r="K91">
+        <v>0</v>
+      </c>
+      <c r="L91">
+        <v>0</v>
+      </c>
+      <c r="M91">
+        <v>0</v>
+      </c>
+      <c r="N91">
+        <v>0</v>
+      </c>
+      <c r="O91">
+        <v>0</v>
+      </c>
+      <c r="P91">
+        <v>0</v>
+      </c>
+      <c r="Q91">
+        <v>0</v>
+      </c>
+      <c r="R91">
+        <v>1</v>
+      </c>
+      <c r="S91" s="3" t="str">
+        <f>DEC2HEX(C91*2^15 + D91*2^14 + E91*2^13 + F91*2^12 + G91*2^11 + H91*2^10 + I91*2^9 + J91*2^8 + K91*2^7 + L91*2^6 + M91*2^5 + N91*2^4 + O91 * 2 ^ 3 + P91  * 2^2 + Q91 * 2 + R91)</f>
+        <v>601</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>166</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+      <c r="D92">
+        <v>0</v>
+      </c>
+      <c r="E92">
+        <v>0</v>
+      </c>
+      <c r="F92">
+        <v>1</v>
+      </c>
+      <c r="G92">
+        <v>0</v>
+      </c>
+      <c r="H92">
+        <v>0</v>
+      </c>
+      <c r="I92">
+        <v>1</v>
+      </c>
+      <c r="J92">
+        <v>1</v>
+      </c>
+      <c r="K92">
+        <v>1</v>
+      </c>
+      <c r="L92">
+        <v>1</v>
+      </c>
+      <c r="M92">
+        <v>0</v>
+      </c>
+      <c r="N92">
+        <v>0</v>
+      </c>
+      <c r="O92">
+        <v>0</v>
+      </c>
+      <c r="P92">
+        <v>0</v>
+      </c>
+      <c r="Q92">
+        <v>0</v>
+      </c>
+      <c r="R92">
+        <v>0</v>
+      </c>
+      <c r="S92" s="3" t="str">
+        <f t="shared" ref="S92:S97" si="6">DEC2HEX(C92*2^15 + D92*2^14 + E92*2^13 + F92*2^12 + G92*2^11 + H92*2^10 + I92*2^9 + J92*2^8 + K92*2^7 + L92*2^6 + M92*2^5 + N92*2^4 + O92 * 2 ^ 3 + P92  * 2^2 + Q92 * 2 + R92)</f>
+        <v>13C0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>167</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+      <c r="E93">
+        <v>0</v>
+      </c>
+      <c r="F93">
+        <v>1</v>
+      </c>
+      <c r="G93">
+        <v>1</v>
+      </c>
+      <c r="H93">
+        <v>0</v>
+      </c>
+      <c r="I93">
+        <v>1</v>
+      </c>
+      <c r="J93">
+        <v>1</v>
+      </c>
+      <c r="K93">
+        <v>1</v>
+      </c>
+      <c r="L93">
+        <v>0</v>
+      </c>
+      <c r="M93">
+        <v>0</v>
+      </c>
+      <c r="N93">
+        <v>0</v>
+      </c>
+      <c r="O93">
+        <v>0</v>
+      </c>
+      <c r="P93">
+        <v>0</v>
+      </c>
+      <c r="Q93">
+        <v>0</v>
+      </c>
+      <c r="R93">
+        <v>0</v>
+      </c>
+      <c r="S93" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>1B80</v>
+      </c>
+    </row>
+    <row r="94" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>168</v>
+      </c>
+      <c r="B94" t="s">
+        <v>131</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+      <c r="E94">
+        <v>0</v>
+      </c>
+      <c r="F94">
+        <v>1</v>
+      </c>
+      <c r="G94">
+        <v>0</v>
+      </c>
+      <c r="H94">
+        <v>1</v>
+      </c>
+      <c r="I94">
+        <v>0</v>
+      </c>
+      <c r="J94">
+        <v>1</v>
+      </c>
+      <c r="K94">
+        <v>0</v>
+      </c>
+      <c r="L94">
+        <v>0</v>
+      </c>
+      <c r="M94">
+        <v>1</v>
+      </c>
+      <c r="N94">
+        <v>0</v>
+      </c>
+      <c r="O94">
+        <v>0</v>
+      </c>
+      <c r="P94">
+        <v>0</v>
+      </c>
+      <c r="Q94">
+        <v>1</v>
+      </c>
+      <c r="R94">
+        <v>1</v>
+      </c>
+      <c r="S94" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>1523</v>
+      </c>
+    </row>
+    <row r="95" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>169</v>
+      </c>
+      <c r="B95" t="s">
+        <v>95</v>
+      </c>
+      <c r="C95">
+        <v>0</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+      <c r="E95">
+        <v>0</v>
+      </c>
+      <c r="F95">
+        <v>1</v>
+      </c>
+      <c r="G95">
+        <v>0</v>
+      </c>
+      <c r="H95">
+        <v>0</v>
+      </c>
+      <c r="I95">
+        <v>1</v>
+      </c>
+      <c r="J95">
+        <v>1</v>
+      </c>
+      <c r="K95">
+        <v>0</v>
+      </c>
+      <c r="L95">
+        <v>0</v>
+      </c>
+      <c r="M95">
+        <v>0</v>
+      </c>
+      <c r="N95">
+        <v>0</v>
+      </c>
+      <c r="O95">
+        <v>0</v>
+      </c>
+      <c r="P95">
+        <v>0</v>
+      </c>
+      <c r="Q95">
+        <v>0</v>
+      </c>
+      <c r="R95">
+        <v>0</v>
+      </c>
+      <c r="S95" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="96" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>170</v>
+      </c>
+      <c r="B96" t="s">
+        <v>186</v>
+      </c>
+      <c r="C96">
+        <v>1</v>
+      </c>
+      <c r="D96">
+        <v>1</v>
+      </c>
+      <c r="E96">
+        <v>0</v>
+      </c>
+      <c r="F96">
+        <v>0</v>
+      </c>
+      <c r="G96">
+        <v>1</v>
+      </c>
+      <c r="H96">
+        <v>1</v>
+      </c>
+      <c r="I96">
+        <v>1</v>
+      </c>
+      <c r="J96">
+        <v>0</v>
+      </c>
+      <c r="K96">
+        <v>0</v>
+      </c>
+      <c r="L96">
+        <v>0</v>
+      </c>
+      <c r="M96">
+        <v>0</v>
+      </c>
+      <c r="N96">
+        <v>0</v>
+      </c>
+      <c r="O96">
+        <v>1</v>
+      </c>
+      <c r="P96">
+        <v>1</v>
+      </c>
+      <c r="Q96">
+        <v>0</v>
+      </c>
+      <c r="R96">
+        <v>0</v>
+      </c>
+      <c r="S96" s="3" t="str">
+        <f>DEC2HEX(C96*2^15 + D96*2^14 + E96*2^13 + F96*2^12 + G96*2^11 + H96*2^10 + I96*2^9 + J96*2^8 + K96*2^7 + L96*2^6 + M96*2^5 + N96*2^4 + O96 * 2 ^ 3 + P96  * 2^2 + Q96 * 2 + R96)</f>
+        <v>CE0C</v>
+      </c>
+    </row>
+    <row r="97" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>171</v>
+      </c>
+      <c r="B97" t="s">
+        <v>101</v>
+      </c>
+      <c r="C97">
+        <v>0</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+      <c r="E97">
+        <v>0</v>
+      </c>
+      <c r="F97">
+        <v>0</v>
+      </c>
+      <c r="G97">
+        <v>0</v>
+      </c>
+      <c r="H97">
+        <v>0</v>
+      </c>
+      <c r="I97">
+        <v>0</v>
+      </c>
+      <c r="J97">
+        <v>1</v>
+      </c>
+      <c r="K97">
+        <v>0</v>
+      </c>
+      <c r="L97">
+        <v>1</v>
+      </c>
+      <c r="M97">
+        <v>0</v>
+      </c>
+      <c r="N97">
+        <v>0</v>
+      </c>
+      <c r="O97">
+        <v>0</v>
+      </c>
+      <c r="P97">
+        <v>1</v>
+      </c>
+      <c r="Q97">
+        <v>1</v>
+      </c>
+      <c r="R97">
+        <v>1</v>
+      </c>
+      <c r="S97" s="3" t="str">
+        <f>DEC2HEX(C97*2^15 + D97*2^14 + E97*2^13 + F97*2^12 + G97*2^11 + H97*2^10 + I97*2^9 + J97*2^8 + K97*2^7 + L97*2^6 + M97*2^5 + N97*2^4 + O97 * 2 ^ 3 + P97  * 2^2 + Q97 * 2 + R97)</f>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="98" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>172</v>
+      </c>
+      <c r="B98" t="s">
+        <v>102</v>
+      </c>
+      <c r="C98">
+        <v>0</v>
+      </c>
+      <c r="D98">
+        <v>0</v>
+      </c>
+      <c r="E98">
+        <v>0</v>
+      </c>
+      <c r="F98">
+        <v>0</v>
+      </c>
+      <c r="G98">
+        <v>0</v>
+      </c>
+      <c r="H98">
+        <v>1</v>
+      </c>
+      <c r="I98">
+        <v>0</v>
+      </c>
+      <c r="J98">
+        <v>0</v>
+      </c>
+      <c r="K98">
+        <v>0</v>
+      </c>
+      <c r="L98">
+        <v>0</v>
+      </c>
+      <c r="M98">
+        <v>0</v>
+      </c>
+      <c r="N98">
+        <v>0</v>
+      </c>
+      <c r="O98">
+        <v>0</v>
+      </c>
+      <c r="P98">
+        <v>0</v>
+      </c>
+      <c r="Q98">
+        <v>1</v>
+      </c>
+      <c r="R98">
+        <v>1</v>
+      </c>
+      <c r="S98" s="3" t="str">
+        <f>DEC2HEX(C98*2^15 + D98*2^14 + E98*2^13 + F98*2^12 + G98*2^11 + H98*2^10 + I98*2^9 + J98*2^8 + K98*2^7 + L98*2^6 + M98*2^5 + N98*2^4 + O98 * 2 ^ 3 + P98  * 2^2 + Q98 * 2 + R98)</f>
+        <v>403</v>
+      </c>
+    </row>
+    <row r="99" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>185</v>
+      </c>
+      <c r="B99" t="s">
+        <v>45</v>
+      </c>
+      <c r="C99">
+        <v>0</v>
+      </c>
+      <c r="D99">
+        <v>1</v>
+      </c>
+      <c r="E99">
+        <v>1</v>
+      </c>
+      <c r="F99">
+        <v>1</v>
+      </c>
+      <c r="G99">
+        <v>0</v>
+      </c>
+      <c r="H99">
+        <v>0</v>
+      </c>
+      <c r="I99">
+        <v>0</v>
+      </c>
+      <c r="J99">
+        <v>0</v>
+      </c>
+      <c r="K99">
+        <v>0</v>
+      </c>
+      <c r="L99">
+        <v>0</v>
+      </c>
+      <c r="M99">
+        <v>0</v>
+      </c>
+      <c r="N99">
+        <v>0</v>
+      </c>
+      <c r="O99">
+        <v>0</v>
+      </c>
+      <c r="P99">
+        <v>0</v>
+      </c>
+      <c r="Q99">
+        <v>0</v>
+      </c>
+      <c r="R99">
+        <v>0</v>
+      </c>
+      <c r="S99" s="3" t="str">
+        <f>DEC2HEX(C99*2^15 + D99*2^14 + E99*2^13 + F99*2^12 + G99*2^11 + H99*2^10 + I99*2^9 + J99*2^8 + K99*2^7 + L99*2^6 + M99*2^5 + N99*2^4 + O99 * 2 ^ 3 + P99  * 2^2 + Q99 * 2 + R99)</f>
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="100" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S100" s="3"/>
+    </row>
+    <row r="101" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S101" s="3"/>
+    </row>
+    <row r="102" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S102" s="3"/>
+    </row>
+    <row r="103" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S103" s="3"/>
+    </row>
+    <row r="104" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S104" s="3"/>
+    </row>
+    <row r="105" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S105" s="3"/>
+    </row>
+    <row r="106" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S106" s="3"/>
+    </row>
+    <row r="107" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S107" s="3"/>
+    </row>
+    <row r="108" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S108" s="3"/>
+    </row>
+    <row r="109" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S109" s="3"/>
+    </row>
+    <row r="110" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S110" s="3"/>
+    </row>
+    <row r="111" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S111" s="3"/>
+    </row>
+    <row r="112" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S112" s="3"/>
+    </row>
+    <row r="113" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S113" s="3"/>
+    </row>
+    <row r="115" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S115" s="3"/>
+    </row>
+    <row r="116" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B116" s="5"/>
+      <c r="S116" s="3"/>
+    </row>
+    <row r="117" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S117" s="3"/>
+    </row>
+    <row r="118" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S118" s="3"/>
+    </row>
+    <row r="119" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S119" s="3"/>
+    </row>
+    <row r="123" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S123" s="3"/>
+    </row>
+    <row r="124" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S124" s="3"/>
+    </row>
+    <row r="125" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S125" s="3"/>
+    </row>
+    <row r="126" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S126" s="3"/>
+    </row>
+    <row r="127" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A127" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B127" t="s">
+        <v>45</v>
+      </c>
+      <c r="C127">
+        <v>0</v>
+      </c>
+      <c r="D127">
+        <v>1</v>
+      </c>
+      <c r="E127">
+        <v>1</v>
+      </c>
+      <c r="F127">
+        <v>1</v>
+      </c>
+      <c r="G127">
+        <v>0</v>
+      </c>
+      <c r="H127">
+        <v>0</v>
+      </c>
+      <c r="I127">
+        <v>0</v>
+      </c>
+      <c r="J127">
+        <v>0</v>
+      </c>
+      <c r="K127">
+        <v>0</v>
+      </c>
+      <c r="L127">
+        <v>0</v>
+      </c>
+      <c r="M127">
+        <v>0</v>
+      </c>
+      <c r="N127">
+        <v>0</v>
+      </c>
+      <c r="O127">
+        <v>0</v>
+      </c>
+      <c r="P127">
+        <v>0</v>
+      </c>
+      <c r="Q127">
+        <v>0</v>
+      </c>
+      <c r="R127">
+        <v>0</v>
+      </c>
+      <c r="S127" s="3" t="str">
+        <f>DEC2HEX(C127*2^15 + D127*2^14 + E127*2^13 + F127*2^12 + G127*2^11 + H127*2^10 + I127*2^9 + J127*2^8 + K127*2^7 + L127*2^6 + M127*2^5 + N127*2^4 + O127 * 2 ^ 3 + P127  * 2^2 + Q127 * 2 + R127)</f>
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="128" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>23</v>
+      </c>
+      <c r="B128" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C128" s="6">
+        <v>0</v>
+      </c>
+      <c r="D128" s="7">
+        <v>0</v>
+      </c>
+      <c r="E128" s="7">
+        <v>0</v>
+      </c>
+      <c r="F128" s="7">
+        <v>0</v>
+      </c>
+      <c r="G128" s="7">
+        <v>1</v>
+      </c>
+      <c r="H128" s="7">
+        <v>1</v>
+      </c>
+      <c r="I128" s="7">
+        <v>1</v>
+      </c>
+      <c r="J128" s="7">
+        <v>1</v>
+      </c>
+      <c r="K128" s="7">
+        <v>1</v>
+      </c>
+      <c r="L128" s="7">
+        <v>1</v>
+      </c>
+      <c r="M128" s="7">
+        <v>0</v>
+      </c>
+      <c r="N128" s="7">
+        <v>1</v>
+      </c>
+      <c r="O128" s="7">
+        <v>1</v>
+      </c>
+      <c r="P128" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q128" s="7">
+        <v>1</v>
+      </c>
+      <c r="R128" s="7">
+        <v>1</v>
+      </c>
+      <c r="S128" s="3" t="str">
+        <f>DEC2HEX(C128*2^15 + D128*2^14 + E128*2^13 + F128*2^12 + G128*2^11 + H128*2^10 + I128*2^9 + J128*2^8 + K128*2^7 + L128*2^6 + M128*2^5 + N128*2^4 + O128 * 2 ^ 3 + P128  * 2^2 + Q128 * 2 + R128)</f>
+        <v>FDB</v>
+      </c>
+    </row>
+    <row r="129" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>24</v>
+      </c>
+      <c r="B129" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C129">
+        <v>0</v>
+      </c>
+      <c r="D129">
+        <v>0</v>
+      </c>
+      <c r="E129">
+        <v>1</v>
+      </c>
+      <c r="F129">
+        <v>1</v>
+      </c>
+      <c r="G129">
+        <v>1</v>
+      </c>
+      <c r="H129">
+        <v>1</v>
+      </c>
+      <c r="I129">
+        <v>1</v>
+      </c>
+      <c r="J129">
+        <v>1</v>
+      </c>
+      <c r="K129">
+        <v>1</v>
+      </c>
+      <c r="L129">
+        <v>1</v>
+      </c>
+      <c r="M129">
+        <v>0</v>
+      </c>
+      <c r="N129">
+        <v>0</v>
+      </c>
+      <c r="O129">
+        <v>1</v>
+      </c>
+      <c r="P129">
+        <v>0</v>
+      </c>
+      <c r="Q129">
+        <v>0</v>
+      </c>
+      <c r="R129">
+        <v>1</v>
+      </c>
+      <c r="S129" s="3" t="str">
+        <f t="shared" ref="S129:S131" si="7">DEC2HEX(C129*2^15 + D129*2^14 + E129*2^13 + F129*2^12 + G129*2^11 + H129*2^10 + I129*2^9 + J129*2^8 + K129*2^7 + L129*2^6 + M129*2^5 + N129*2^4 + O129 * 2 ^ 3 + P129  * 2^2 + Q129 * 2 + R129)</f>
+        <v>3FC9</v>
+      </c>
+    </row>
+    <row r="130" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>25</v>
+      </c>
+      <c r="B130" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C130" s="7">
+        <v>1</v>
+      </c>
+      <c r="D130" s="7">
+        <v>0</v>
+      </c>
+      <c r="E130" s="7">
+        <v>1</v>
+      </c>
+      <c r="F130" s="7">
+        <v>0</v>
+      </c>
+      <c r="G130" s="7">
+        <v>1</v>
+      </c>
+      <c r="H130" s="7">
+        <v>0</v>
+      </c>
+      <c r="I130" s="7">
+        <v>1</v>
+      </c>
+      <c r="J130" s="7">
+        <v>0</v>
+      </c>
+      <c r="K130" s="7">
+        <v>1</v>
+      </c>
+      <c r="L130" s="7">
+        <v>0</v>
+      </c>
+      <c r="M130" s="7">
+        <v>1</v>
+      </c>
+      <c r="N130" s="7">
+        <v>0</v>
+      </c>
+      <c r="O130" s="7">
+        <v>1</v>
+      </c>
+      <c r="P130" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q130" s="7">
+        <v>1</v>
+      </c>
+      <c r="R130" s="7">
+        <v>1</v>
+      </c>
+      <c r="S130" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>AAAB</v>
+      </c>
+    </row>
+    <row r="131" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>26</v>
+      </c>
+      <c r="B131" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C131" s="7">
+        <v>0</v>
+      </c>
+      <c r="D131" s="7">
+        <v>0</v>
+      </c>
+      <c r="E131" s="7">
+        <v>1</v>
+      </c>
+      <c r="F131" s="7">
+        <v>1</v>
+      </c>
+      <c r="G131" s="7">
+        <v>1</v>
+      </c>
+      <c r="H131" s="7">
+        <v>1</v>
+      </c>
+      <c r="I131" s="7">
+        <v>1</v>
+      </c>
+      <c r="J131" s="7">
+        <v>0</v>
+      </c>
+      <c r="K131" s="7">
+        <v>0</v>
+      </c>
+      <c r="L131" s="7">
+        <v>0</v>
+      </c>
+      <c r="M131" s="7">
+        <v>1</v>
+      </c>
+      <c r="N131" s="7">
+        <v>0</v>
+      </c>
+      <c r="O131" s="7">
+        <v>1</v>
+      </c>
+      <c r="P131" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q131" s="7">
+        <v>1</v>
+      </c>
+      <c r="R131" s="7">
+        <v>0</v>
+      </c>
+      <c r="S131" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>3E2A</v>
+      </c>
+    </row>
+    <row r="132" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>27</v>
+      </c>
+      <c r="B132" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="133" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>28</v>
+      </c>
+      <c r="B133" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="134" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>29</v>
+      </c>
+      <c r="B134" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C134" s="7">
+        <v>1</v>
+      </c>
+      <c r="D134" s="7">
+        <v>0</v>
+      </c>
+      <c r="E134" s="7">
+        <v>0</v>
+      </c>
+      <c r="F134" s="7">
+        <v>0</v>
+      </c>
+      <c r="G134" s="7">
+        <v>1</v>
+      </c>
+      <c r="H134" s="7">
+        <v>0</v>
+      </c>
+      <c r="I134" s="7">
+        <v>0</v>
+      </c>
+      <c r="J134" s="7">
+        <v>0</v>
+      </c>
+      <c r="K134" s="7">
+        <v>1</v>
+      </c>
+      <c r="L134" s="7">
+        <v>0</v>
+      </c>
+      <c r="M134" s="7">
+        <v>0</v>
+      </c>
+      <c r="N134" s="7">
+        <v>0</v>
+      </c>
+      <c r="O134" s="7">
+        <v>1</v>
+      </c>
+      <c r="P134" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q134" s="7">
+        <v>0</v>
+      </c>
+      <c r="R134" s="7">
+        <v>1</v>
+      </c>
+      <c r="S134" s="3" t="str">
+        <f t="shared" ref="S134:S135" si="8">DEC2HEX(C134*2^15 + D134*2^14 + E134*2^13 + F134*2^12 + G134*2^11 + H134*2^10 + I134*2^9 + J134*2^8 + K134*2^7 + L134*2^6 + M134*2^5 + N134*2^4 + O134 * 2 ^ 3 + P134  * 2^2 + Q134 * 2 + R134)</f>
+        <v>8889</v>
+      </c>
+    </row>
+    <row r="135" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>30</v>
+      </c>
+      <c r="B135" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C135" s="7">
+        <v>0</v>
+      </c>
+      <c r="D135" s="7">
+        <v>0</v>
+      </c>
+      <c r="E135" s="7">
+        <v>1</v>
+      </c>
+      <c r="F135" s="7">
+        <v>1</v>
+      </c>
+      <c r="G135" s="7">
+        <v>1</v>
+      </c>
+      <c r="H135" s="7">
+        <v>1</v>
+      </c>
+      <c r="I135" s="7">
+        <v>0</v>
+      </c>
+      <c r="J135" s="7">
+        <v>0</v>
+      </c>
+      <c r="K135" s="7">
+        <v>0</v>
+      </c>
+      <c r="L135" s="7">
+        <v>0</v>
+      </c>
+      <c r="M135" s="7">
+        <v>0</v>
+      </c>
+      <c r="N135" s="7">
+        <v>0</v>
+      </c>
+      <c r="O135" s="7">
+        <v>1</v>
+      </c>
+      <c r="P135" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q135" s="7">
+        <v>0</v>
+      </c>
+      <c r="R135" s="7">
+        <v>0</v>
+      </c>
+      <c r="S135" s="3" t="str">
+        <f t="shared" si="8"/>
         <v>3C08</v>
       </c>
     </row>
-    <row r="84" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
+    <row r="136" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
         <v>31</v>
       </c>
-      <c r="B84" s="14" t="s">
+      <c r="B136" s="14" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="85" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
+    <row r="137" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
         <v>32</v>
       </c>
-      <c r="B85" s="14" t="s">
+      <c r="B137" s="14" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="86" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
+    <row r="138" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
         <v>38</v>
       </c>
-      <c r="B86" s="14" t="s">
+      <c r="B138" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="C86" s="7">
-        <v>0</v>
-      </c>
-      <c r="D86" s="7">
-        <v>0</v>
-      </c>
-      <c r="E86" s="7">
-        <v>0</v>
-      </c>
-      <c r="F86" s="7">
-        <v>0</v>
-      </c>
-      <c r="G86" s="7">
-        <v>1</v>
-      </c>
-      <c r="H86" s="7">
-        <v>1</v>
-      </c>
-      <c r="I86" s="7">
-        <v>0</v>
-      </c>
-      <c r="J86" s="7">
-        <v>1</v>
-      </c>
-      <c r="K86" s="7">
-        <v>0</v>
-      </c>
-      <c r="L86" s="7">
-        <v>0</v>
-      </c>
-      <c r="M86" s="7">
-        <v>0</v>
-      </c>
-      <c r="N86" s="7">
-        <v>0</v>
-      </c>
-      <c r="O86" s="7">
-        <v>0</v>
-      </c>
-      <c r="P86" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q86" s="7">
-        <v>0</v>
-      </c>
-      <c r="R86" s="7">
-        <v>0</v>
-      </c>
-      <c r="S86" s="3">
+      <c r="C138" s="7">
+        <v>0</v>
+      </c>
+      <c r="D138" s="7">
+        <v>0</v>
+      </c>
+      <c r="E138" s="7">
+        <v>0</v>
+      </c>
+      <c r="F138" s="7">
+        <v>0</v>
+      </c>
+      <c r="G138" s="7">
+        <v>1</v>
+      </c>
+      <c r="H138" s="7">
+        <v>1</v>
+      </c>
+      <c r="I138" s="7">
+        <v>0</v>
+      </c>
+      <c r="J138" s="7">
+        <v>1</v>
+      </c>
+      <c r="K138" s="7">
+        <v>0</v>
+      </c>
+      <c r="L138" s="7">
+        <v>0</v>
+      </c>
+      <c r="M138" s="7">
+        <v>0</v>
+      </c>
+      <c r="N138" s="7">
+        <v>0</v>
+      </c>
+      <c r="O138" s="7">
+        <v>0</v>
+      </c>
+      <c r="P138" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q138" s="7">
+        <v>0</v>
+      </c>
+      <c r="R138" s="7">
+        <v>0</v>
+      </c>
+      <c r="S138" s="3">
         <v>1400</v>
       </c>
-      <c r="T86" t="s">
+      <c r="T138" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="87" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
+    <row r="139" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
         <v>39</v>
       </c>
-      <c r="B87" s="14" t="s">
+      <c r="B139" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="C87" s="7">
-        <v>0</v>
-      </c>
-      <c r="D87" s="7">
-        <v>0</v>
-      </c>
-      <c r="E87" s="7">
-        <v>1</v>
-      </c>
-      <c r="F87" s="7">
-        <v>1</v>
-      </c>
-      <c r="G87" s="7">
-        <v>1</v>
-      </c>
-      <c r="H87" s="7">
-        <v>0</v>
-      </c>
-      <c r="I87" s="7">
-        <v>0</v>
-      </c>
-      <c r="J87" s="7">
-        <v>1</v>
-      </c>
-      <c r="K87" s="7">
-        <v>0</v>
-      </c>
-      <c r="L87" s="7">
-        <v>1</v>
-      </c>
-      <c r="M87" s="7">
-        <v>0</v>
-      </c>
-      <c r="N87" s="7">
-        <v>1</v>
-      </c>
-      <c r="O87" s="7">
-        <v>0</v>
-      </c>
-      <c r="P87" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q87" s="7">
-        <v>0</v>
-      </c>
-      <c r="R87" s="7">
-        <v>0</v>
-      </c>
-      <c r="S87" s="3" t="str">
-        <f t="shared" ref="S87" si="5">DEC2HEX(C87*2^15 + D87*2^14 + E87*2^13 + F87*2^12 + G87*2^11 + H87*2^10 + I87*2^9 + J87*2^8 + K87*2^7 + L87*2^6 + M87*2^5 + N87*2^4 + O87 * 2 ^ 3 + P87  * 2^2 + Q87 * 2 + R87)</f>
+      <c r="C139" s="7">
+        <v>0</v>
+      </c>
+      <c r="D139" s="7">
+        <v>0</v>
+      </c>
+      <c r="E139" s="7">
+        <v>1</v>
+      </c>
+      <c r="F139" s="7">
+        <v>1</v>
+      </c>
+      <c r="G139" s="7">
+        <v>1</v>
+      </c>
+      <c r="H139" s="7">
+        <v>0</v>
+      </c>
+      <c r="I139" s="7">
+        <v>0</v>
+      </c>
+      <c r="J139" s="7">
+        <v>1</v>
+      </c>
+      <c r="K139" s="7">
+        <v>0</v>
+      </c>
+      <c r="L139" s="7">
+        <v>1</v>
+      </c>
+      <c r="M139" s="7">
+        <v>0</v>
+      </c>
+      <c r="N139" s="7">
+        <v>1</v>
+      </c>
+      <c r="O139" s="7">
+        <v>0</v>
+      </c>
+      <c r="P139" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q139" s="7">
+        <v>0</v>
+      </c>
+      <c r="R139" s="7">
+        <v>0</v>
+      </c>
+      <c r="S139" s="3" t="str">
+        <f t="shared" ref="S139" si="9">DEC2HEX(C139*2^15 + D139*2^14 + E139*2^13 + F139*2^12 + G139*2^11 + H139*2^10 + I139*2^9 + J139*2^8 + K139*2^7 + L139*2^6 + M139*2^5 + N139*2^4 + O139 * 2 ^ 3 + P139  * 2^2 + Q139 * 2 + R139)</f>
         <v>3950</v>
       </c>
-      <c r="T87" t="s">
+      <c r="T139" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="88" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
+    <row r="140" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
         <v>40</v>
       </c>
-      <c r="B88" s="14" t="s">
+      <c r="B140" s="14" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="89" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
+    <row r="141" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
         <v>41</v>
       </c>
-      <c r="B89" s="14" t="s">
+      <c r="B141" s="14" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="90" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
+    <row r="142" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
         <v>42</v>
       </c>
-      <c r="B90" s="14" t="s">
+      <c r="B142" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="C90">
-        <v>1</v>
-      </c>
-      <c r="D90">
-        <v>1</v>
-      </c>
-      <c r="E90">
-        <v>1</v>
-      </c>
-      <c r="F90">
-        <v>0</v>
-      </c>
-      <c r="G90">
-        <v>1</v>
-      </c>
-      <c r="H90">
-        <v>1</v>
-      </c>
-      <c r="I90">
-        <v>1</v>
-      </c>
-      <c r="J90">
-        <v>1</v>
-      </c>
-      <c r="K90">
-        <v>0</v>
-      </c>
-      <c r="L90">
-        <v>0</v>
-      </c>
-      <c r="M90">
-        <v>0</v>
-      </c>
-      <c r="N90">
-        <v>1</v>
-      </c>
-      <c r="O90">
-        <v>0</v>
-      </c>
-      <c r="P90">
-        <v>1</v>
-      </c>
-      <c r="Q90">
-        <v>0</v>
-      </c>
-      <c r="R90">
-        <v>1</v>
-      </c>
-      <c r="S90" s="3" t="str">
-        <f t="shared" ref="S90:S91" si="6">DEC2HEX(C90*2^15 + D90*2^14 + E90*2^13 + F90*2^12 + G90*2^11 + H90*2^10 + I90*2^9 + J90*2^8 + K90*2^7 + L90*2^6 + M90*2^5 + N90*2^4 + O90 * 2 ^ 3 + P90  * 2^2 + Q90 * 2 + R90)</f>
+      <c r="C142">
+        <v>1</v>
+      </c>
+      <c r="D142">
+        <v>1</v>
+      </c>
+      <c r="E142">
+        <v>1</v>
+      </c>
+      <c r="F142">
+        <v>0</v>
+      </c>
+      <c r="G142">
+        <v>1</v>
+      </c>
+      <c r="H142">
+        <v>1</v>
+      </c>
+      <c r="I142">
+        <v>1</v>
+      </c>
+      <c r="J142">
+        <v>1</v>
+      </c>
+      <c r="K142">
+        <v>0</v>
+      </c>
+      <c r="L142">
+        <v>0</v>
+      </c>
+      <c r="M142">
+        <v>0</v>
+      </c>
+      <c r="N142">
+        <v>1</v>
+      </c>
+      <c r="O142">
+        <v>0</v>
+      </c>
+      <c r="P142">
+        <v>1</v>
+      </c>
+      <c r="Q142">
+        <v>0</v>
+      </c>
+      <c r="R142">
+        <v>1</v>
+      </c>
+      <c r="S142" s="3" t="str">
+        <f t="shared" ref="S142:S143" si="10">DEC2HEX(C142*2^15 + D142*2^14 + E142*2^13 + F142*2^12 + G142*2^11 + H142*2^10 + I142*2^9 + J142*2^8 + K142*2^7 + L142*2^6 + M142*2^5 + N142*2^4 + O142 * 2 ^ 3 + P142  * 2^2 + Q142 * 2 + R142)</f>
         <v>EF15</v>
       </c>
     </row>
-    <row r="91" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
+    <row r="143" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
         <v>43</v>
       </c>
-      <c r="B91" s="14" t="s">
+      <c r="B143" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="C91">
-        <v>0</v>
-      </c>
-      <c r="D91">
-        <v>0</v>
-      </c>
-      <c r="E91">
-        <v>1</v>
-      </c>
-      <c r="F91">
-        <v>1</v>
-      </c>
-      <c r="G91">
-        <v>0</v>
-      </c>
-      <c r="H91">
-        <v>1</v>
-      </c>
-      <c r="I91">
-        <v>1</v>
-      </c>
-      <c r="J91">
-        <v>0</v>
-      </c>
-      <c r="K91">
-        <v>0</v>
-      </c>
-      <c r="L91">
-        <v>0</v>
-      </c>
-      <c r="M91">
-        <v>1</v>
-      </c>
-      <c r="N91">
-        <v>1</v>
-      </c>
-      <c r="O91">
-        <v>1</v>
-      </c>
-      <c r="P91">
-        <v>0</v>
-      </c>
-      <c r="Q91">
-        <v>0</v>
-      </c>
-      <c r="R91">
-        <v>0</v>
-      </c>
-      <c r="S91" s="3" t="str">
-        <f t="shared" si="6"/>
+      <c r="C143">
+        <v>0</v>
+      </c>
+      <c r="D143">
+        <v>0</v>
+      </c>
+      <c r="E143">
+        <v>1</v>
+      </c>
+      <c r="F143">
+        <v>1</v>
+      </c>
+      <c r="G143">
+        <v>0</v>
+      </c>
+      <c r="H143">
+        <v>1</v>
+      </c>
+      <c r="I143">
+        <v>1</v>
+      </c>
+      <c r="J143">
+        <v>0</v>
+      </c>
+      <c r="K143">
+        <v>0</v>
+      </c>
+      <c r="L143">
+        <v>0</v>
+      </c>
+      <c r="M143">
+        <v>1</v>
+      </c>
+      <c r="N143">
+        <v>1</v>
+      </c>
+      <c r="O143">
+        <v>1</v>
+      </c>
+      <c r="P143">
+        <v>0</v>
+      </c>
+      <c r="Q143">
+        <v>0</v>
+      </c>
+      <c r="R143">
+        <v>0</v>
+      </c>
+      <c r="S143" s="3" t="str">
+        <f t="shared" si="10"/>
         <v>3638</v>
       </c>
     </row>
-    <row r="92" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
+    <row r="144" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
         <v>33</v>
       </c>
-      <c r="B92" s="14" t="s">
+      <c r="B144" s="14" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="93" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
+    <row r="145" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
         <v>82</v>
       </c>
-      <c r="B93" s="14" t="s">
+      <c r="B145" s="14" t="s">
         <v>75</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N2:R2"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="K3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="A8:V8"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="Q7:R7"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="M4:P4"/>
     <mergeCell ref="I6:J6"/>
@@ -5256,21 +7717,6 @@
     <mergeCell ref="I5:R5"/>
     <mergeCell ref="C6:F6"/>
     <mergeCell ref="G6:H6"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="A8:V8"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N2:R2"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="K3:N3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:R3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5607,7 +8053,7 @@
         <v>30</v>
       </c>
       <c r="B10">
-        <f>Code!B71</f>
+        <f>Code!B123</f>
         <v>0</v>
       </c>
       <c r="C10" t="str">
@@ -5632,11 +8078,11 @@
         <v>31</v>
       </c>
       <c r="B11">
-        <f>Code!B72</f>
+        <f>Code!B124</f>
         <v>0</v>
       </c>
       <c r="C11">
-        <f>Code!S71</f>
+        <f>Code!S123</f>
         <v>0</v>
       </c>
       <c r="Q11" t="s">
@@ -5657,11 +8103,11 @@
         <v>32</v>
       </c>
       <c r="B12">
-        <f>Code!B73</f>
+        <f>Code!B125</f>
         <v>0</v>
       </c>
       <c r="C12">
-        <f>Code!S72</f>
+        <f>Code!S124</f>
         <v>0</v>
       </c>
       <c r="S12" t="s">
@@ -5686,7 +8132,7 @@
         <v>0x02D</v>
       </c>
       <c r="C13">
-        <f>Code!S73</f>
+        <f>Code!S125</f>
         <v>0</v>
       </c>
       <c r="U13" t="s">
@@ -5707,11 +8153,11 @@
         <v>39</v>
       </c>
       <c r="B14" t="str">
-        <f>Code!B75</f>
+        <f>Code!B127</f>
         <v>STP</v>
       </c>
       <c r="C14">
-        <f>Code!S74</f>
+        <f>Code!S126</f>
         <v>0</v>
       </c>
       <c r="W14" t="s">
@@ -5736,7 +8182,7 @@
         <v>#REF!</v>
       </c>
       <c r="C15" t="str">
-        <f>Code!S75</f>
+        <f>Code!S127</f>
         <v>7000</v>
       </c>
       <c r="Y15" t="s">

</xml_diff>

<commit_message>
docs(fpu): add program for testing the FPU #2
</commit_message>
<xml_diff>
--- a/programs/fpumaclaurinprogramsinpiover2-32bits.xlsx
+++ b/programs/fpumaclaurinprogramsinpiover2-32bits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vacla\Projects\cpu\programs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE0E5BD-F5B8-43AF-8054-B93BAB91356E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E701DDBA-1702-468C-8658-8F80A52DDD1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E410B2C1-F054-41C4-A96D-F1120FBD95E0}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="187">
   <si>
     <t>Hex</t>
   </si>
@@ -1002,8 +1002,8 @@
   <dimension ref="A1:AK145"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K98" sqref="K98"/>
+      <pane ySplit="8" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K102" sqref="K102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6467,7 +6467,7 @@
         <v>0</v>
       </c>
       <c r="S92" s="3" t="str">
-        <f t="shared" ref="S92:S97" si="6">DEC2HEX(C92*2^15 + D92*2^14 + E92*2^13 + F92*2^12 + G92*2^11 + H92*2^10 + I92*2^9 + J92*2^8 + K92*2^7 + L92*2^6 + M92*2^5 + N92*2^4 + O92 * 2 ^ 3 + P92  * 2^2 + Q92 * 2 + R92)</f>
+        <f t="shared" ref="S92:S95" si="6">DEC2HEX(C92*2^15 + D92*2^14 + E92*2^13 + F92*2^12 + G92*2^11 + H92*2^10 + I92*2^9 + J92*2^8 + K92*2^7 + L92*2^6 + M92*2^5 + N92*2^4 + O92 * 2 ^ 3 + P92  * 2^2 + Q92 * 2 + R92)</f>
         <v>13C0</v>
       </c>
     </row>
@@ -6965,61 +6965,7 @@
       <c r="A127" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="B127" t="s">
-        <v>45</v>
-      </c>
-      <c r="C127">
-        <v>0</v>
-      </c>
-      <c r="D127">
-        <v>1</v>
-      </c>
-      <c r="E127">
-        <v>1</v>
-      </c>
-      <c r="F127">
-        <v>1</v>
-      </c>
-      <c r="G127">
-        <v>0</v>
-      </c>
-      <c r="H127">
-        <v>0</v>
-      </c>
-      <c r="I127">
-        <v>0</v>
-      </c>
-      <c r="J127">
-        <v>0</v>
-      </c>
-      <c r="K127">
-        <v>0</v>
-      </c>
-      <c r="L127">
-        <v>0</v>
-      </c>
-      <c r="M127">
-        <v>0</v>
-      </c>
-      <c r="N127">
-        <v>0</v>
-      </c>
-      <c r="O127">
-        <v>0</v>
-      </c>
-      <c r="P127">
-        <v>0</v>
-      </c>
-      <c r="Q127">
-        <v>0</v>
-      </c>
-      <c r="R127">
-        <v>0</v>
-      </c>
-      <c r="S127" s="3" t="str">
-        <f>DEC2HEX(C127*2^15 + D127*2^14 + E127*2^13 + F127*2^12 + G127*2^11 + H127*2^10 + I127*2^9 + J127*2^8 + K127*2^7 + L127*2^6 + M127*2^5 + N127*2^4 + O127 * 2 ^ 3 + P127  * 2^2 + Q127 * 2 + R127)</f>
-        <v>7000</v>
-      </c>
+      <c r="S127" s="3"/>
     </row>
     <row r="128" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
@@ -7692,21 +7638,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N2:R2"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="K3:N3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="A8:V8"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="Q7:R7"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="M4:P4"/>
     <mergeCell ref="I6:J6"/>
@@ -7717,6 +7648,21 @@
     <mergeCell ref="I5:R5"/>
     <mergeCell ref="C6:F6"/>
     <mergeCell ref="G6:H6"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="A8:V8"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N2:R2"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="K3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8152,9 +8098,9 @@
       <c r="A14" t="s">
         <v>39</v>
       </c>
-      <c r="B14" t="str">
+      <c r="B14">
         <f>Code!B127</f>
-        <v>STP</v>
+        <v>0</v>
       </c>
       <c r="C14">
         <f>Code!S126</f>
@@ -8181,9 +8127,9 @@
         <f>Code!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="C15" t="str">
+      <c r="C15">
         <f>Code!S127</f>
-        <v>7000</v>
+        <v>0</v>
       </c>
       <c r="Y15" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
feat(fpu): multiplier change operands of the multiplier #28
</commit_message>
<xml_diff>
--- a/programs/fpumaclaurinprogramsinpiover2-32bits.xlsx
+++ b/programs/fpumaclaurinprogramsinpiover2-32bits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vacla\Projects\cpu\programs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF49125-08AB-48EF-9965-A2EE70ABEB02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F078752C-7ACB-421F-B757-45A29B283C83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E410B2C1-F054-41C4-A96D-F1120FBD95E0}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="187">
   <si>
     <t>Hex</t>
   </si>
@@ -999,11 +999,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E17FB6-AC76-4C3E-BEFA-6AB3607784FD}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AK145"/>
+  <dimension ref="A1:AK147"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M83" sqref="M83"/>
+      <pane ySplit="8" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H128" sqref="H128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7203,7 +7203,7 @@
         <v>0</v>
       </c>
       <c r="S131" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f>DEC2HEX(C131*2^15 + D131*2^14 + E131*2^13 + F131*2^12 + G131*2^11 + H131*2^10 + I131*2^9 + J131*2^8 + K131*2^7 + L131*2^6 + M131*2^5 + N131*2^4 + O131 * 2 ^ 3 + P131  * 2^2 + Q131 * 2 + R131)</f>
         <v>3E2A</v>
       </c>
     </row>
@@ -7630,10 +7630,20 @@
     </row>
     <row r="145" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B145" s="14" t="s">
         <v>75</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(fpu): add carry save adder for the mantissa addition #28
</commit_message>
<xml_diff>
--- a/programs/fpumaclaurinprogramsinpiover2-32bits.xlsx
+++ b/programs/fpumaclaurinprogramsinpiover2-32bits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vacla\Projects\cpu\programs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F078752C-7ACB-421F-B757-45A29B283C83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BE2E6E-CDC2-43E4-8DCE-7F2FEC88E41D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E410B2C1-F054-41C4-A96D-F1120FBD95E0}"/>
   </bookViews>
@@ -1003,7 +1003,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H128" sqref="H128"/>
+      <selection pane="bottomLeft" activeCell="N136" sqref="N136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7083,7 +7083,7 @@
         <v>1</v>
       </c>
       <c r="S129" s="3" t="str">
-        <f t="shared" ref="S129:S131" si="7">DEC2HEX(C129*2^15 + D129*2^14 + E129*2^13 + F129*2^12 + G129*2^11 + H129*2^10 + I129*2^9 + J129*2^8 + K129*2^7 + L129*2^6 + M129*2^5 + N129*2^4 + O129 * 2 ^ 3 + P129  * 2^2 + Q129 * 2 + R129)</f>
+        <f t="shared" ref="S129:S130" si="7">DEC2HEX(C129*2^15 + D129*2^14 + E129*2^13 + F129*2^12 + G129*2^11 + H129*2^10 + I129*2^9 + J129*2^8 + K129*2^7 + L129*2^6 + M129*2^5 + N129*2^4 + O129 * 2 ^ 3 + P129  * 2^2 + Q129 * 2 + R129)</f>
         <v>3FC9</v>
       </c>
     </row>
@@ -7648,21 +7648,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N2:R2"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="K3:N3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="A8:V8"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="Q7:R7"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="M4:P4"/>
     <mergeCell ref="I6:J6"/>
@@ -7673,6 +7658,21 @@
     <mergeCell ref="I5:R5"/>
     <mergeCell ref="C6:F6"/>
     <mergeCell ref="G6:H6"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="A8:V8"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N2:R2"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="K3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>